<commit_message>
finished editing excels and doing comparison graphs
</commit_message>
<xml_diff>
--- a/batch2.xlsx
+++ b/batch2.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mackenzieobrien/mlc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE39D887-B13E-A446-B3F1-7043C20F7D0E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A0789E-C3A4-684B-831F-B795DF13F8A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="920" windowWidth="27640" windowHeight="15220" xr2:uid="{AC62FFA5-95F4-E649-B7DA-2DBEF876D547}"/>
+    <workbookView xWindow="14440" yWindow="0" windowWidth="14360" windowHeight="18000" xr2:uid="{AC62FFA5-95F4-E649-B7DA-2DBEF876D547}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$1</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="40">
   <si>
     <t>chewy</t>
   </si>
@@ -69,15 +72,6 @@
     <t>taylor.vanderbiezen1@marist.edu</t>
   </si>
   <si>
-    <t>roger.norton@marist.edu</t>
-  </si>
-  <si>
-    <t>65-74</t>
-  </si>
-  <si>
-    <t>louis.kavouras1@marist.edu</t>
-  </si>
-  <si>
     <t>Yes, email me the details</t>
   </si>
   <si>
@@ -129,25 +123,7 @@
     <t>Erin.holder2@marist.edu</t>
   </si>
   <si>
-    <t>Kate.tashjian1@marist.edu</t>
-  </si>
-  <si>
     <t>Matthew.oakley1@marist.edu</t>
-  </si>
-  <si>
-    <t>chewy, gooey</t>
-  </si>
-  <si>
-    <t>matthew.oakley1@marist.edu</t>
-  </si>
-  <si>
-    <t>alex/mahlmeister1@marist.edu</t>
-  </si>
-  <si>
-    <t>alexander.mosiychuk1</t>
-  </si>
-  <si>
-    <t>timothy.zwart1@marist.edu</t>
   </si>
   <si>
     <t>michael.presta1@marist.edu</t>
@@ -536,70 +512,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B31882-748B-2946-AF62-B61256EE22B7}">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="G1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -610,31 +586,31 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -645,57 +621,53 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1">
         <v>5</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1">
         <v>9</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>2</v>
@@ -704,7 +676,7 @@
         <v>7</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -715,34 +687,38 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -755,22 +731,22 @@
         <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E7" s="1">
         <v>9</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -781,28 +757,28 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>4</v>
@@ -822,25 +798,25 @@
         <v>5</v>
       </c>
       <c r="C9" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E9" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -851,10 +827,10 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="1">
         <v>5</v>
@@ -863,19 +839,19 @@
         <v>0</v>
       </c>
       <c r="E10" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -886,31 +862,31 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1">
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E11" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -921,31 +897,31 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B12" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E12" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -956,7 +932,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B13" s="1">
         <v>4</v>
@@ -965,19 +941,19 @@
         <v>5</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E13" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>4</v>
@@ -991,31 +967,31 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E14" s="1">
         <v>9</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1026,31 +1002,31 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B15" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C15" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="E15" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -1061,31 +1037,31 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B16" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C16" s="1">
         <v>5</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E16" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="G16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -1096,31 +1072,31 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B17" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C17" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="1">
         <v>8</v>
       </c>
-      <c r="E17" s="1">
-        <v>5</v>
-      </c>
       <c r="F17" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -1131,31 +1107,31 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E18" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -1166,22 +1142,22 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B19" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C19" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E19" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>2</v>
@@ -1201,25 +1177,25 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C20" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E20" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>7</v>
@@ -1234,252 +1210,12 @@
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>3</v>
-      </c>
-      <c r="B21" s="1">
-        <v>4</v>
-      </c>
-      <c r="C21" s="1">
-        <v>4</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E21" s="1">
-        <v>7</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>5</v>
-      </c>
-      <c r="B22" s="1">
-        <v>4</v>
-      </c>
-      <c r="C22" s="1">
-        <v>5</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="1">
-        <v>9</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>5</v>
-      </c>
-      <c r="B23" s="1">
-        <v>4</v>
-      </c>
-      <c r="C23" s="1">
-        <v>5</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E23" s="1">
-        <v>8</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>4</v>
-      </c>
-      <c r="B24" s="1">
-        <v>4</v>
-      </c>
-      <c r="C24" s="1">
-        <v>4</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="1">
-        <v>7</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>5</v>
-      </c>
-      <c r="B25" s="1">
-        <v>5</v>
-      </c>
-      <c r="C25" s="1">
-        <v>5</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E25" s="1">
-        <v>8</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>4</v>
-      </c>
-      <c r="B26" s="1">
-        <v>3</v>
-      </c>
-      <c r="C26" s="1">
-        <v>3</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E26" s="1">
-        <v>5</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>4</v>
-      </c>
-      <c r="B27" s="1">
-        <v>4</v>
-      </c>
-      <c r="C27" s="1">
-        <v>5</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E27" s="1">
-        <v>9</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:I1" xr:uid="{7B45F344-647E-EC49-8F7C-8B4590651B07}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I20">
+      <sortCondition ref="F1:F20"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>